<commit_message>
DESCW-1283 add template and partial model
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_6_rpt_CA_ConsultingServiceUtilization-FY-Summary-by Portfolio.xlsx
+++ b/backend/reports/xlsx/Tab_6_rpt_CA_ConsultingServiceUtilization-FY-Summary-by Portfolio.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACD1F40-CB51-3446-9A60-66AD8848772E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD91BED-74CB-3246-AF82-FBA933E01BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>{#date=d.date}</t>
   </si>
@@ -60,15 +60,9 @@
     <t>Resource Type</t>
   </si>
   <si>
-    <t>BCS</t>
-  </si>
-  <si>
     <t>OSS</t>
   </si>
   <si>
-    <t>SIPS</t>
-  </si>
-  <si>
     <t>DP</t>
   </si>
   <si>
@@ -78,17 +72,68 @@
     <t>DMS</t>
   </si>
   <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
     <t>{$rows}</t>
+  </si>
+  <si>
+    <t>{$row.resource_type}</t>
+  </si>
+  <si>
+    <t>BCF</t>
+  </si>
+  <si>
+    <t>{$row.bcf}</t>
+  </si>
+  <si>
+    <t>{$row.oss}</t>
+  </si>
+  <si>
+    <t>{$row.des}</t>
+  </si>
+  <si>
+    <t>DES</t>
+  </si>
+  <si>
+    <t>{$row.dp}</t>
+  </si>
+  <si>
+    <t>{$row.ana}</t>
+  </si>
+  <si>
+    <t>{$row.dms}</t>
+  </si>
+  <si>
+    <t>{$row.sd}</t>
+  </si>
+  <si>
+    <t>{$row.ce}</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>{$row.gc}</t>
+  </si>
+  <si>
+    <t>{$row.total}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,8 +160,16 @@
       <sz val="10"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,12 +185,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,7 +298,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,7 +681,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -669,27 +716,35 @@
         <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="J2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
@@ -697,12 +752,44 @@
       <c r="P2" s="9"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" ht="17" thickBot="1">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -713,20 +800,24 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="K4" s="13"/>
       <c r="L4" s="5"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+    <row r="5" spans="1:16" ht="17" thickBot="1">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="9" spans="1:16" ht="17">
       <c r="B9" s="8" t="s">

</xml_diff>

<commit_message>
descw-1283 updates model and template
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_6_rpt_CA_ConsultingServiceUtilization-FY-Summary-by Portfolio.xlsx
+++ b/backend/reports/xlsx/Tab_6_rpt_CA_ConsultingServiceUtilization-FY-Summary-by Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD91BED-74CB-3246-AF82-FBA933E01BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D9FAEA-D8C9-ED48-92D4-0512CFBC3AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-2880" yWindow="-19260" windowWidth="29920" windowHeight="18660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>{#date=d.date}</t>
   </si>
@@ -127,13 +127,43 @@
   </si>
   <si>
     <t>{$row.total}</t>
+  </si>
+  <si>
+    <t>{$totals.bcf}</t>
+  </si>
+  <si>
+    <t>{$totals.oss}</t>
+  </si>
+  <si>
+    <t>{$totals.des}</t>
+  </si>
+  <si>
+    <t>{$totals.dp}</t>
+  </si>
+  <si>
+    <t>{$totals.ana}</t>
+  </si>
+  <si>
+    <t>{$totals.dms}</t>
+  </si>
+  <si>
+    <t>{$totals.sd}</t>
+  </si>
+  <si>
+    <t>{$totals.ce}</t>
+  </si>
+  <si>
+    <t>{$totals.gc}</t>
+  </si>
+  <si>
+    <t>{$totals.total}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -164,6 +194,21 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -299,6 +344,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +728,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -689,6 +736,7 @@
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="79" customHeight="1" thickBot="1">
@@ -808,16 +856,36 @@
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="B5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="17">
       <c r="B9" s="8" t="s">

</xml_diff>